<commit_message>
Finally got last page number in bot.py
</commit_message>
<xml_diff>
--- a/input_data/input_data.xlsx
+++ b/input_data/input_data.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/85b56c852a094943/Python Projects/cslb_bot-1/input_data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/85b56c852a094943/Python Projects/cslb_bot-2/input_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="11" documentId="8_{EA09F524-A56F-42D3-9F07-8A512D6FC85C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{632E5201-FDDB-42B7-8014-4DCA4E90826C}"/>
+  <xr:revisionPtr revIDLastSave="18" documentId="8_{EA09F524-A56F-42D3-9F07-8A512D6FC85C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{B3D1DFA3-04EE-4A60-9DA6-C3859251DA7F}"/>
   <bookViews>
     <workbookView xWindow="840" yWindow="-120" windowWidth="20880" windowHeight="13740" xr2:uid="{4073E3CB-9528-4FB7-ACBF-798F9A191E58}"/>
   </bookViews>
@@ -34,24 +34,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
     <t>B - General Building Contractor</t>
   </si>
   <si>
     <t>Temecula</t>
-  </si>
-  <si>
-    <t>lake elsinore</t>
-  </si>
-  <si>
-    <t>escondido</t>
-  </si>
-  <si>
-    <t>Murry</t>
-  </si>
-  <si>
-    <t>HH</t>
   </si>
 </sst>
 </file>
@@ -403,10 +391,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32419621-F59E-45C4-B6BD-D6AB737F794D}">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="A2" sqref="A2:B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -423,31 +411,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
-        <v>0</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Successful in getting all license numbers in a list.
</commit_message>
<xml_diff>
--- a/input_data/input_data.xlsx
+++ b/input_data/input_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/85b56c852a094943/Python Projects/cslb_bot-2/input_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="18" documentId="8_{EA09F524-A56F-42D3-9F07-8A512D6FC85C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{B3D1DFA3-04EE-4A60-9DA6-C3859251DA7F}"/>
+  <xr:revisionPtr revIDLastSave="23" documentId="8_{EA09F524-A56F-42D3-9F07-8A512D6FC85C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{34347364-5A41-4C85-B3BF-4B0E05535D17}"/>
   <bookViews>
     <workbookView xWindow="840" yWindow="-120" windowWidth="20880" windowHeight="13740" xr2:uid="{4073E3CB-9528-4FB7-ACBF-798F9A191E58}"/>
   </bookViews>
@@ -393,9 +393,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32419621-F59E-45C4-B6BD-D6AB737F794D}">
   <dimension ref="A1:B1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:B4"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>

<commit_message>
modify bot.py and bot2.py
</commit_message>
<xml_diff>
--- a/input_data/input_data.xlsx
+++ b/input_data/input_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/85b56c852a094943/Python Projects/cslb_bot-2/input_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="23" documentId="8_{EA09F524-A56F-42D3-9F07-8A512D6FC85C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{34347364-5A41-4C85-B3BF-4B0E05535D17}"/>
+  <xr:revisionPtr revIDLastSave="24" documentId="8_{EA09F524-A56F-42D3-9F07-8A512D6FC85C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{9C281024-4EDF-4776-B870-8CF09038D528}"/>
   <bookViews>
     <workbookView xWindow="840" yWindow="-120" windowWidth="20880" windowHeight="13740" xr2:uid="{4073E3CB-9528-4FB7-ACBF-798F9A191E58}"/>
   </bookViews>
@@ -39,7 +39,7 @@
     <t>B - General Building Contractor</t>
   </si>
   <si>
-    <t>Temecula</t>
+    <t>TEMECULA</t>
   </si>
 </sst>
 </file>

</xml_diff>